<commit_message>
add test for fdo#75168
Change-Id: Iffb07d98333667837a7a2bba00e2d667d49bb709
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/new_cond_format_test.xlsx
+++ b/sc/qa/unit/data/xlsx/new_cond_format_test.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xlsx\conditional format\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="10725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -89,45 +85,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -433,7 +396,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,7 +406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
@@ -1023,28 +986,78 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="top10" dxfId="14" priority="8" rank="5"/>
+    <cfRule type="top10" dxfId="13" priority="8" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D22">
-    <cfRule type="top10" dxfId="13" priority="7" bottom="1" rank="5"/>
+    <cfRule type="top10" dxfId="12" priority="7" bottom="1" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
-    <cfRule type="top10" dxfId="12" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H22">
-    <cfRule type="top10" dxfId="11" priority="5" percent="1" bottom="1" rank="15"/>
+    <cfRule type="top10" dxfId="10" priority="5" percent="1" bottom="1" rank="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J22">
-    <cfRule type="aboveAverage" dxfId="10" priority="4"/>
+    <cfRule type="aboveAverage" dxfId="9" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L22">
-    <cfRule type="aboveAverage" dxfId="4" priority="3" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="8" priority="3" aboveAverage="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N22">
-    <cfRule type="aboveAverage" dxfId="3" priority="2" equalAverage="1"/>
+    <cfRule type="aboveAverage" dxfId="7" priority="2" equalAverage="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P22">
-    <cfRule type="aboveAverage" dxfId="1" priority="1" aboveAverage="0" equalAverage="1"/>
+    <cfRule type="aboveAverage" dxfId="6" priority="1" aboveAverage="0" equalAverage="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A3">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>A1&lt;&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B3">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>B1=1</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>